<commit_message>
added support for "abort" results from Uppaal in the reports; improved the hammer example
</commit_message>
<xml_diff>
--- a/examples/hammer/hammer.xlsx
+++ b/examples/hammer/hammer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jose/Documents/Research/projects/valu3s/wip/uppx/examples/hammer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1196E08B-38CC-014E-A6EB-96AE47B59C91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B64EE1-3474-3948-B358-0A35CF77759D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21200" windowHeight="12980" activeTab="3" xr2:uid="{F23A7857-2A5B-744A-861E-37E01B360061}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21200" windowHeight="12980" xr2:uid="{F23A7857-2A5B-744A-861E-37E01B360061}"/>
   </bookViews>
   <sheets>
     <sheet name="@Configurations" sheetId="15" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="224">
   <si>
     <t>Comment</t>
   </si>
@@ -73,13 +73,7 @@
     <t>worker starts working</t>
   </si>
   <si>
-    <t>totalHits</t>
-  </si>
-  <si>
     <t>workingTime</t>
-  </si>
-  <si>
-    <t>Total number of hits before the hammer stops working</t>
   </si>
   <si>
     <t>Total time that the worker can work before stopping</t>
@@ -694,13 +688,31 @@
     <t>CountNails</t>
   </si>
   <si>
-    <t>!Count</t>
-  </si>
-  <si>
     <t>would overflow "nails" when checking</t>
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>totalNails</t>
+  </si>
+  <si>
+    <t>Total number of new nails available (when counting nails)</t>
+  </si>
+  <si>
+    <t>SlowCount</t>
+  </si>
+  <si>
+    <t>infiniteNails</t>
+  </si>
+  <si>
+    <t>If there is no bound on the number of nails (can cause overflows)</t>
+  </si>
+  <si>
+    <t>InfNails</t>
+  </si>
+  <si>
+    <t>InfiniteCount</t>
   </si>
 </sst>
 </file>
@@ -1137,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB81B79D-84CB-DC47-B910-0DBDA508B944}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1146,29 +1158,33 @@
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
     <col min="2" max="4" width="3.33203125" customWidth="1"/>
     <col min="5" max="5" width="3" customWidth="1"/>
+    <col min="6" max="6" width="2.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="55" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="F1" s="9"/>
+        <v>213</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -1188,10 +1204,10 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -1210,11 +1226,11 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -1232,24 +1248,24 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
@@ -1266,13 +1282,13 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -1287,10 +1303,19 @@
       <c r="P7" s="10"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B8" s="10"/>
+      <c r="A8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>179</v>
+      </c>
       <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="D8" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>179</v>
+      </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -1304,11 +1329,18 @@
       <c r="P8" s="10"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>223</v>
+      </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
+      <c r="E9" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>179</v>
+      </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
@@ -1501,7 +1533,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -1509,13 +1541,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1523,15 +1555,15 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>185</v>
+      </c>
+      <c r="C6" t="s">
         <v>187</v>
-      </c>
-      <c r="C6" t="s">
-        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -1545,7 +1577,7 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1573,140 +1605,163 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="5">
+        <v>100</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2">
+        <v>200</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="5">
-        <v>50</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
       <c r="E5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="2">
-        <v>200</v>
+        <v>190</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>192</v>
-      </c>
-      <c r="B7">
-        <v>20</v>
+        <v>190</v>
+      </c>
+      <c r="B7" s="2">
+        <v>150</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>193</v>
+        <v>191</v>
+      </c>
+      <c r="E7" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>192</v>
-      </c>
-      <c r="B8" s="2">
-        <v>150</v>
+        <v>210</v>
+      </c>
+      <c r="B8" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>1</v>
+        <v>211</v>
       </c>
       <c r="D8" t="s">
-        <v>193</v>
-      </c>
-      <c r="E8" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D9" t="s">
         <v>212</v>
       </c>
-      <c r="B9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="E9" t="s">
         <v>213</v>
-      </c>
-      <c r="D9" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>212</v>
-      </c>
-      <c r="B10" s="2" t="b">
+        <v>217</v>
+      </c>
+      <c r="B10" s="2">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>213</v>
-      </c>
       <c r="D10" t="s">
-        <v>214</v>
-      </c>
-      <c r="E10" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
+      <c r="A11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D11" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="A12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D12" t="s">
+        <v>221</v>
+      </c>
+      <c r="E12" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="2"/>
@@ -1725,7 +1780,7 @@
       <c r="C16" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:Y100">
+  <conditionalFormatting sqref="A13:Y100 A3:Y10 C11:E11 A11:A12 C12:Y12">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>_xlfn.ISFORMULA(A3)</formula>
     </cfRule>
@@ -1738,8 +1793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E766410-42AB-D842-913C-A2316B1EA100}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1751,108 +1806,102 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" t="s">
         <v>175</v>
       </c>
-      <c r="B3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C3" t="s">
-        <v>177</v>
-      </c>
-      <c r="D3" t="s">
-        <v>217</v>
-      </c>
       <c r="E3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" t="s">
         <v>197</v>
-      </c>
-      <c r="B5" t="s">
-        <v>198</v>
-      </c>
-      <c r="C5" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B7" t="s">
         <v>201</v>
       </c>
-      <c r="B7" t="s">
-        <v>203</v>
-      </c>
       <c r="C7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" t="s">
+        <v>203</v>
+      </c>
+      <c r="C8" t="s">
         <v>204</v>
       </c>
-      <c r="B8" t="s">
-        <v>205</v>
-      </c>
-      <c r="C8" t="s">
-        <v>206</v>
-      </c>
-      <c r="D8" t="s">
-        <v>217</v>
-      </c>
       <c r="E8" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -1870,227 +1919,227 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
@@ -2100,527 +2149,527 @@
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
@@ -2630,42 +2679,42 @@
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2683,12 +2732,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DA12DE6878FEE740AAE11B8EF5A3BEB8" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ccf3f071624932fa9b6b142dc8790e1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf33d030-a745-437b-8efe-493a0e84c7f1" xmlns:ns3="38766943-c6ee-43fb-a1f1-f050a673c741" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46fa4806b78295368f283e4cef5efe23" ns2:_="" ns3:_="">
     <xsd:import namespace="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
@@ -2899,6 +2942,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A07F53CA-6B4E-4B2E-8600-AB0859BD2077}">
   <ds:schemaRefs>
@@ -2908,23 +2957,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CA45778-FFDE-4083-BC23-84F816C77BB8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38766943-c6ee-43fb-a1f1-f050a673c741"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030D8A7F-6A3B-4D41-86D3-C760184B49E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2941,4 +2973,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CA45778-FFDE-4083-BC23-84F816C77BB8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38766943-c6ee-43fb-a1f1-f050a673c741"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added support for feature model (not exploiting attributes yet, but with some support)
</commit_message>
<xml_diff>
--- a/examples/hammer/hammer.xlsx
+++ b/examples/hammer/hammer.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jose/Documents/Research/projects/valu3s/wip/uppx/examples/hammer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B64EE1-3474-3948-B358-0A35CF77759D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11ED97C9-CF73-AC44-837A-858F0610DC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21200" windowHeight="12980" xr2:uid="{F23A7857-2A5B-744A-861E-37E01B360061}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21200" windowHeight="12980" activeTab="1" xr2:uid="{F23A7857-2A5B-744A-861E-37E01B360061}"/>
   </bookViews>
   <sheets>
     <sheet name="@Configurations" sheetId="15" r:id="rId1"/>
-    <sheet name="@Channels" sheetId="12" r:id="rId2"/>
-    <sheet name="@Limits" sheetId="6" r:id="rId3"/>
-    <sheet name="&lt;queries&gt;" sheetId="14" r:id="rId4"/>
-    <sheet name="AvailableFunctions" sheetId="13" r:id="rId5"/>
+    <sheet name="@FeatureModel" sheetId="16" r:id="rId2"/>
+    <sheet name="@Channels" sheetId="12" r:id="rId3"/>
+    <sheet name="@Limits" sheetId="6" r:id="rId4"/>
+    <sheet name="&lt;queries&gt;" sheetId="14" r:id="rId5"/>
+    <sheet name="AvailableFunctions" sheetId="13" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="231">
   <si>
     <t>Comment</t>
   </si>
@@ -658,9 +659,6 @@
     <t>The worker must be able to rest after working</t>
   </si>
   <si>
-    <t>Never</t>
-  </si>
-  <si>
     <t>Overwork</t>
   </si>
   <si>
@@ -713,13 +711,37 @@
   </si>
   <si>
     <t>InfiniteCount</t>
+  </si>
+  <si>
+    <t>#constraint !(Lazy &amp; Overworker)</t>
+  </si>
+  <si>
+    <t>Hammer</t>
+  </si>
+  <si>
+    <t>Hammer-stat</t>
+  </si>
+  <si>
+    <t>Worker-stat</t>
+  </si>
+  <si>
+    <t>#optional Worker-stat.*</t>
+  </si>
+  <si>
+    <t>Nails</t>
+  </si>
+  <si>
+    <t>#optional Hammer.*</t>
+  </si>
+  <si>
+    <t>#optional InfNails</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -751,8 +773,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -771,6 +807,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -784,7 +844,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -812,6 +872,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1149,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB81B79D-84CB-DC47-B910-0DBDA508B944}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1172,13 +1244,13 @@
         <v>183</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G1" s="9"/>
     </row>
@@ -1226,7 +1298,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10" t="s">
@@ -1248,7 +1320,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>179</v>
@@ -1260,7 +1332,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -1282,7 +1354,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -1304,7 +1376,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>179</v>
@@ -1330,7 +1402,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -1499,6 +1571,102 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5B459A-3BB1-EB4C-924B-0D3FED2B4C76}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="13"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="13"/>
+      <c r="B3" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="13"/>
+      <c r="B4" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44A7D45-3D37-034F-A1FB-B28B84ABA07F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -1571,13 +1739,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16772568-7503-3B4E-B82C-A26E56E7827F}">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1684,43 +1852,43 @@
         <v>191</v>
       </c>
       <c r="E7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>211</v>
-      </c>
-      <c r="D8" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B9" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D9" t="s">
         <v>211</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>212</v>
-      </c>
-      <c r="E9" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B10" s="2">
         <v>5</v>
@@ -1729,38 +1897,38 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B12" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D12" t="s">
+        <v>220</v>
+      </c>
+      <c r="E12" t="s">
         <v>221</v>
-      </c>
-      <c r="E12" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1789,12 +1957,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E766410-42AB-D842-913C-A2316B1EA100}">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1823,7 +1991,7 @@
         <v>180</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1837,7 +2005,7 @@
         <v>175</v>
       </c>
       <c r="E3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1850,9 +2018,6 @@
       <c r="C4" t="s">
         <v>193</v>
       </c>
-      <c r="D4" t="s">
-        <v>205</v>
-      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1870,7 +2035,7 @@
         <v>181</v>
       </c>
       <c r="B6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C6" t="s">
         <v>198</v>
@@ -1901,7 +2066,7 @@
         <v>204</v>
       </c>
       <c r="E8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -1909,7 +2074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC6D41BA-2AFD-1444-8964-7539D3436D4A}">
   <dimension ref="A1:A160"/>
   <sheetViews>
@@ -2723,15 +2888,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DA12DE6878FEE740AAE11B8EF5A3BEB8" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ccf3f071624932fa9b6b142dc8790e1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf33d030-a745-437b-8efe-493a0e84c7f1" xmlns:ns3="38766943-c6ee-43fb-a1f1-f050a673c741" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46fa4806b78295368f283e4cef5efe23" ns2:_="" ns3:_="">
     <xsd:import namespace="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
@@ -2942,21 +3098,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A07F53CA-6B4E-4B2E-8600-AB0859BD2077}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030D8A7F-6A3B-4D41-86D3-C760184B49E7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2975,7 +3132,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CA45778-FFDE-4083-BC23-84F816C77BB8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -2990,4 +3147,12 @@
     <ds:schemaRef ds:uri="38766943-c6ee-43fb-a1f1-f050a673c741"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A07F53CA-6B4E-4B2E-8600-AB0859BD2077}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
improved feature model - more errors detected and better messages
</commit_message>
<xml_diff>
--- a/examples/hammer/hammer.xlsx
+++ b/examples/hammer/hammer.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jose/Documents/Research/projects/valu3s/wip/uppx/examples/hammer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11ED97C9-CF73-AC44-837A-858F0610DC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152D3F4D-58E2-7C45-BC75-722093EB26C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="21200" windowHeight="12980" activeTab="1" xr2:uid="{F23A7857-2A5B-744A-861E-37E01B360061}"/>
   </bookViews>
   <sheets>
     <sheet name="@Configurations" sheetId="15" r:id="rId1"/>
-    <sheet name="@FeatureModel" sheetId="16" r:id="rId2"/>
+    <sheet name="FeatureModel" sheetId="16" r:id="rId2"/>
     <sheet name="@Channels" sheetId="12" r:id="rId3"/>
     <sheet name="@Limits" sheetId="6" r:id="rId4"/>
     <sheet name="&lt;queries&gt;" sheetId="14" r:id="rId5"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="234">
   <si>
     <t>Comment</t>
   </si>
@@ -713,9 +713,6 @@
     <t>InfiniteCount</t>
   </si>
   <si>
-    <t>#constraint !(Lazy &amp; Overworker)</t>
-  </si>
-  <si>
     <t>Hammer</t>
   </si>
   <si>
@@ -735,6 +732,18 @@
   </si>
   <si>
     <t>#optional InfNails</t>
+  </si>
+  <si>
+    <t>$Count</t>
+  </si>
+  <si>
+    <t>#constraint Slow || !Slow</t>
+  </si>
+  <si>
+    <t>#constraint !(Lazy &amp;&amp; Overworker)</t>
+  </si>
+  <si>
+    <t>Count &amp;&amp; !InfNails</t>
   </si>
 </sst>
 </file>
@@ -1222,7 +1231,7 @@
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1359,8 +1368,8 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="E7" s="10" t="s">
-        <v>179</v>
+      <c r="E7" s="10">
+        <v>4</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -1385,8 +1394,8 @@
       <c r="D8" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>179</v>
+      <c r="E8" s="10">
+        <v>3</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
@@ -1407,9 +1416,7 @@
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="10" t="s">
-        <v>179</v>
-      </c>
+      <c r="E9" s="10"/>
       <c r="F9" s="10" t="s">
         <v>179</v>
       </c>
@@ -1572,11 +1579,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5B459A-3BB1-EB4C-924B-0D3FED2B4C76}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1586,10 +1591,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C1" s="16" t="s">
         <v>182</v>
@@ -1605,7 +1610,7 @@
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" s="18" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>206</v>
@@ -1614,7 +1619,7 @@
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
       <c r="B4" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>212</v>
@@ -1635,31 +1640,36 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="12" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>231</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1741,11 +1751,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16772568-7503-3B4E-B82C-A26E56E7827F}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1855,7 +1865,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>209</v>
       </c>
@@ -1891,7 +1901,7 @@
         <v>216</v>
       </c>
       <c r="B10" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>1</v>
@@ -1902,16 +1912,19 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>219</v>
-      </c>
-      <c r="B11" s="2" t="b">
-        <v>0</v>
+        <v>216</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>230</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>210</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>220</v>
+        <v>217</v>
+      </c>
+      <c r="E11" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1919,7 +1932,7 @@
         <v>219</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>210</v>
@@ -1927,13 +1940,23 @@
       <c r="D12" t="s">
         <v>220</v>
       </c>
-      <c r="E12" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>219</v>
+      </c>
+      <c r="B13" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D13" t="s">
+        <v>220</v>
+      </c>
+      <c r="E13" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
@@ -1947,8 +1970,12 @@
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A13:Y100 A3:Y10 C11:E11 A11:A12 C12:Y12">
+  <conditionalFormatting sqref="A14:Y101 C12:E12 A12:A13 C13:Y13 A3:Y11">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>_xlfn.ISFORMULA(A3)</formula>
     </cfRule>
@@ -2888,6 +2915,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DA12DE6878FEE740AAE11B8EF5A3BEB8" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ccf3f071624932fa9b6b142dc8790e1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf33d030-a745-437b-8efe-493a0e84c7f1" xmlns:ns3="38766943-c6ee-43fb-a1f1-f050a673c741" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46fa4806b78295368f283e4cef5efe23" ns2:_="" ns3:_="">
     <xsd:import namespace="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
@@ -3098,36 +3140,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030D8A7F-6A3B-4D41-86D3-C760184B49E7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A07F53CA-6B4E-4B2E-8600-AB0859BD2077}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
-    <ds:schemaRef ds:uri="38766943-c6ee-43fb-a1f1-f050a673c741"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3150,9 +3166,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A07F53CA-6B4E-4B2E-8600-AB0859BD2077}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030D8A7F-6A3B-4D41-86D3-C760184B49E7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
+    <ds:schemaRef ds:uri="38766943-c6ee-43fb-a1f1-f050a673c741"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updating hammer example; improving error messages (timeouts vs. errors)
</commit_message>
<xml_diff>
--- a/examples/hammer/hammer.xlsx
+++ b/examples/hammer/hammer.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jose/Documents/Research/projects/valu3s/wip/uppx/examples/hammer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152D3F4D-58E2-7C45-BC75-722093EB26C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4FD29A3-DDA8-E24D-8DC7-016A76D30DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21200" windowHeight="12980" activeTab="1" xr2:uid="{F23A7857-2A5B-744A-861E-37E01B360061}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21200" windowHeight="12980" activeTab="3" xr2:uid="{F23A7857-2A5B-744A-861E-37E01B360061}"/>
   </bookViews>
   <sheets>
     <sheet name="@Configurations" sheetId="15" r:id="rId1"/>
-    <sheet name="FeatureModel" sheetId="16" r:id="rId2"/>
+    <sheet name="@FeatureModel" sheetId="16" r:id="rId2"/>
     <sheet name="@Channels" sheetId="12" r:id="rId3"/>
     <sheet name="@Limits" sheetId="6" r:id="rId4"/>
     <sheet name="&lt;queries&gt;" sheetId="14" r:id="rId5"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="239">
   <si>
     <t>Comment</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>worker starts working</t>
-  </si>
-  <si>
-    <t>workingTime</t>
   </si>
   <si>
     <t>Total time that the worker can work before stopping</t>
@@ -560,9 +557,6 @@
 &lt;/query&gt;</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>NoDL</t>
   </si>
   <si>
@@ -737,20 +731,41 @@
     <t>$Count</t>
   </si>
   <si>
-    <t>#constraint Slow || !Slow</t>
-  </si>
-  <si>
     <t>#constraint !(Lazy &amp;&amp; Overworker)</t>
   </si>
   <si>
     <t>Count &amp;&amp; !InfNails</t>
+  </si>
+  <si>
+    <t>sessionTime</t>
+  </si>
+  <si>
+    <t>The hammer can complete at least $Count nails</t>
+  </si>
+  <si>
+    <t>The hammer must complete at least $Count nails</t>
+  </si>
+  <si>
+    <t>A&lt;&gt; nails&gt;=$Count</t>
+  </si>
+  <si>
+    <t>Can reach X nails</t>
+  </si>
+  <si>
+    <t>Must reach X nails</t>
+  </si>
+  <si>
+    <t>E&lt;&gt; nails&gt;=$Count</t>
+  </si>
+  <si>
+    <t>Short name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -796,8 +811,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -840,6 +863,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -853,7 +882,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -893,6 +922,24 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1230,8 +1277,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB81B79D-84CB-DC47-B910-0DBDA508B944}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1242,30 +1290,30 @@
     <col min="6" max="6" width="2.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="55" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="10"/>
@@ -1285,10 +1333,10 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -1307,11 +1355,11 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -1329,24 +1377,24 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C5" s="10"/>
       <c r="D5" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
       <c r="D6" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
@@ -1363,7 +1411,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -1385,14 +1433,14 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E8" s="10">
         <v>3</v>
@@ -1411,14 +1459,16 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
+      <c r="E9" s="10">
+        <v>0</v>
+      </c>
       <c r="F9" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
@@ -1579,9 +1629,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5B459A-3BB1-EB4C-924B-0D3FED2B4C76}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1591,50 +1643,52 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>225</v>
-      </c>
       <c r="C1" s="16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="13"/>
       <c r="B2" s="15"/>
       <c r="C2" s="17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" s="18" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
       <c r="B4" s="19" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
+      <c r="A6" s="12" t="s">
+        <v>224</v>
+      </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
     </row>
@@ -1647,7 +1701,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -1660,16 +1714,7 @@
       <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="12" t="s">
-        <v>231</v>
-      </c>
+      <c r="A10" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1680,7 +1725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44A7D45-3D37-034F-A1FB-B28B84ABA07F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1711,7 +1756,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -1719,13 +1764,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1733,15 +1778,15 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C6" t="s">
         <v>185</v>
-      </c>
-      <c r="C6" t="s">
-        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1753,15 +1798,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16772568-7503-3B4E-B82C-A26E56E7827F}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="12.83203125" customWidth="1"/>
-    <col min="4" max="4" width="53.83203125" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="54" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1769,26 +1817,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" s="27" t="s">
         <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>231</v>
       </c>
       <c r="B3" s="5">
         <v>100</v>
@@ -1796,13 +1844,13 @@
       <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
+      <c r="E3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>231</v>
       </c>
       <c r="B4" s="5">
         <v>50</v>
@@ -1811,15 +1859,15 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>180</v>
       </c>
       <c r="E4" t="s">
-        <v>182</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>231</v>
       </c>
       <c r="B5" s="2">
         <v>200</v>
@@ -1828,134 +1876,134 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>181</v>
       </c>
       <c r="E5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>190</v>
-      </c>
-      <c r="B6">
-        <v>20</v>
+        <v>207</v>
+      </c>
+      <c r="B6" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>191</v>
+        <v>208</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>190</v>
-      </c>
-      <c r="B7" s="2">
-        <v>150</v>
+        <v>207</v>
+      </c>
+      <c r="B7" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
-        <v>191</v>
-      </c>
-      <c r="E7" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>209</v>
-      </c>
-      <c r="B8" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>211</v>
+      <c r="E8" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>209</v>
-      </c>
-      <c r="B9" s="2" t="b">
+        <v>214</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="D9" t="s">
-        <v>211</v>
+      <c r="D9" s="25" t="s">
+        <v>230</v>
       </c>
       <c r="E9" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>216</v>
-      </c>
-      <c r="B10" s="2">
+        <v>217</v>
+      </c>
+      <c r="B10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>217</v>
+        <v>208</v>
+      </c>
+      <c r="E10" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>216</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>230</v>
+        <v>217</v>
+      </c>
+      <c r="B11" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>1</v>
+        <v>208</v>
       </c>
       <c r="D11" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="E11" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>219</v>
-      </c>
-      <c r="B12" s="2" t="b">
-        <v>0</v>
+        <v>188</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="D12" t="s">
-        <v>220</v>
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>219</v>
-      </c>
-      <c r="B13" s="2" t="b">
+        <v>188</v>
+      </c>
+      <c r="B13" s="2">
+        <v>50</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>210</v>
-      </c>
       <c r="D13" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="E13" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1975,7 +2023,7 @@
       <c r="C17" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A14:Y101 C12:E12 A12:A13 C13:Y13 A3:Y11">
+  <conditionalFormatting sqref="A10:A13 A14:E101 C10:E13 F11:Y101 A3:Y9 A12:Y13">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>_xlfn.ISFORMULA(A3)</formula>
     </cfRule>
@@ -1986,114 +2034,144 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E766410-42AB-D842-913C-A2316B1EA100}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5" customWidth="1"/>
-    <col min="2" max="2" width="30.83203125" customWidth="1"/>
-    <col min="3" max="3" width="40.1640625" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="42.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C2" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>215</v>
+      <c r="D2" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" t="s">
         <v>173</v>
       </c>
-      <c r="B3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C3" t="s">
-        <v>175</v>
+      <c r="D3" t="s">
+        <v>171</v>
       </c>
       <c r="E3" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>194</v>
-      </c>
-      <c r="B4" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" t="s">
         <v>192</v>
-      </c>
-      <c r="C4" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C5" t="s">
         <v>195</v>
       </c>
-      <c r="B5" t="s">
-        <v>196</v>
-      </c>
-      <c r="C5" t="s">
-        <v>197</v>
+      <c r="D5" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>206</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>180</v>
       </c>
       <c r="C6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>199</v>
       </c>
-      <c r="B7" t="s">
-        <v>201</v>
-      </c>
       <c r="C7" t="s">
-        <v>200</v>
+        <v>198</v>
+      </c>
+      <c r="D7" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C8" t="s">
         <v>202</v>
       </c>
-      <c r="B8" t="s">
-        <v>203</v>
-      </c>
-      <c r="C8" t="s">
-        <v>204</v>
+      <c r="D8" t="s">
+        <v>200</v>
       </c>
       <c r="E8" t="s">
-        <v>214</v>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="B9" t="s">
+        <v>210</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="D9" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="B10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="D10" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2111,227 +2189,227 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
@@ -2341,527 +2419,527 @@
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
@@ -2871,42 +2949,42 @@
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2915,21 +2993,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DA12DE6878FEE740AAE11B8EF5A3BEB8" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ccf3f071624932fa9b6b142dc8790e1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf33d030-a745-437b-8efe-493a0e84c7f1" xmlns:ns3="38766943-c6ee-43fb-a1f1-f050a673c741" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46fa4806b78295368f283e4cef5efe23" ns2:_="" ns3:_="">
     <xsd:import namespace="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
@@ -3140,10 +3203,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A07F53CA-6B4E-4B2E-8600-AB0859BD2077}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030D8A7F-6A3B-4D41-86D3-C760184B49E7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
+    <ds:schemaRef ds:uri="38766943-c6ee-43fb-a1f1-f050a673c741"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3166,20 +3255,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030D8A7F-6A3B-4D41-86D3-C760184B49E7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A07F53CA-6B4E-4B2E-8600-AB0859BD2077}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
-    <ds:schemaRef ds:uri="38766943-c6ee-43fb-a1f1-f050a673c741"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
supporting the validation of configurations without running Uppaal (option --validate)
</commit_message>
<xml_diff>
--- a/examples/hammer/hammer.xlsx
+++ b/examples/hammer/hammer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jose/Documents/Research/projects/valu3s/wip/uppx/examples/hammer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4FD29A3-DDA8-E24D-8DC7-016A76D30DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67C3CD7-FE4C-C64F-90F9-724FFE210B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21200" windowHeight="12980" activeTab="3" xr2:uid="{F23A7857-2A5B-744A-861E-37E01B360061}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21200" windowHeight="12980" xr2:uid="{F23A7857-2A5B-744A-861E-37E01B360061}"/>
   </bookViews>
   <sheets>
     <sheet name="@Configurations" sheetId="15" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="241">
   <si>
     <t>Comment</t>
   </si>
@@ -710,15 +710,6 @@
     <t>Hammer</t>
   </si>
   <si>
-    <t>Hammer-stat</t>
-  </si>
-  <si>
-    <t>Worker-stat</t>
-  </si>
-  <si>
-    <t>#optional Worker-stat.*</t>
-  </si>
-  <si>
     <t>Nails</t>
   </si>
   <si>
@@ -759,6 +750,21 @@
   </si>
   <si>
     <t>Short name</t>
+  </si>
+  <si>
+    <t>Worker-effort</t>
+  </si>
+  <si>
+    <t>Hammer-speed</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>#alternative Worker-effort.*</t>
+  </si>
+  <si>
+    <t>not needed</t>
   </si>
 </sst>
 </file>
@@ -882,7 +888,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -929,15 +935,13 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1277,9 +1281,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB81B79D-84CB-DC47-B910-0DBDA508B944}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD10"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1629,16 +1633,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5B459A-3BB1-EB4C-924B-0D3FED2B4C76}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1646,75 +1650,87 @@
         <v>221</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="C1" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="13"/>
+      <c r="A2" s="14"/>
       <c r="B2" s="15"/>
-      <c r="C2" s="17" t="s">
-        <v>181</v>
+      <c r="C2" s="16" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
-      <c r="B3" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>204</v>
+      <c r="B3" s="15"/>
+      <c r="C3" s="17" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
-      <c r="B4" s="19" t="s">
-        <v>225</v>
-      </c>
-      <c r="C4" s="19" t="s">
+      <c r="B4" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
+      <c r="B5" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D5" s="20" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>224</v>
-      </c>
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="12"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="D12" t="s">
+        <v>240</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1798,7 +1814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16772568-7503-3B4E-B82C-A26E56E7827F}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -1817,7 +1833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
         <v>3</v>
       </c>
@@ -1830,13 +1846,13 @@
       <c r="D2" s="23" t="s">
         <v>178</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="25" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B3" s="5">
         <v>100</v>
@@ -1850,7 +1866,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B4" s="5">
         <v>50</v>
@@ -1867,7 +1883,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B5" s="2">
         <v>200</v>
@@ -1931,14 +1947,14 @@
       <c r="A9" t="s">
         <v>214</v>
       </c>
-      <c r="B9" s="26" t="s">
-        <v>228</v>
+      <c r="B9" s="24" t="s">
+        <v>225</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="25" t="s">
-        <v>230</v>
+      <c r="D9" t="s">
+        <v>227</v>
       </c>
       <c r="E9" t="s">
         <v>215</v>
@@ -2023,7 +2039,7 @@
       <c r="C17" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A10:A13 A14:E101 C10:E13 F11:Y101 A3:Y9 A12:Y13">
+  <conditionalFormatting sqref="A3:Y9 A10:A13 C10:E13 F11:Y101 A12:Y13 A14:E101">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>_xlfn.ISFORMULA(A3)</formula>
     </cfRule>
@@ -2054,20 +2070,20 @@
       </c>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+    <row r="2" spans="1:5" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="27" t="s">
-        <v>238</v>
-      </c>
-      <c r="E2" s="27" t="s">
+      <c r="D2" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="E2" s="25" t="s">
         <v>213</v>
       </c>
     </row>
@@ -2148,30 +2164,30 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B9" t="s">
         <v>210</v>
       </c>
       <c r="C9" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="D9" t="s">
         <v>233</v>
-      </c>
-      <c r="D9" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B10" t="s">
         <v>210</v>
       </c>
       <c r="C10" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="D10" t="s">
         <v>232</v>
-      </c>
-      <c r="D10" t="s">
-        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed: when expanding features the attributes were being overwritten
</commit_message>
<xml_diff>
--- a/examples/hammer/hammer.xlsx
+++ b/examples/hammer/hammer.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jose/Documents/Research/projects/valu3s/wip/uppx/examples/hammer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67C3CD7-FE4C-C64F-90F9-724FFE210B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B81FB6E-8DFD-D644-925D-99A86BEB8086}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21200" windowHeight="12980" xr2:uid="{F23A7857-2A5B-744A-861E-37E01B360061}"/>
+    <workbookView xWindow="7600" yWindow="1800" windowWidth="21200" windowHeight="12980" xr2:uid="{F23A7857-2A5B-744A-861E-37E01B360061}"/>
   </bookViews>
   <sheets>
     <sheet name="@Configurations" sheetId="15" r:id="rId1"/>
-    <sheet name="@FeatureModel" sheetId="16" r:id="rId2"/>
-    <sheet name="@Channels" sheetId="12" r:id="rId3"/>
-    <sheet name="@Limits" sheetId="6" r:id="rId4"/>
-    <sheet name="&lt;queries&gt;" sheetId="14" r:id="rId5"/>
+    <sheet name="@Limits" sheetId="6" r:id="rId2"/>
+    <sheet name="&lt;queries&gt;" sheetId="14" r:id="rId3"/>
+    <sheet name="@FeatureModel" sheetId="16" r:id="rId4"/>
+    <sheet name="@Channels" sheetId="12" r:id="rId5"/>
     <sheet name="AvailableFunctions" sheetId="13" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -677,9 +677,6 @@
     <t>Count</t>
   </si>
   <si>
-    <t>CountNails</t>
-  </si>
-  <si>
     <t>would overflow "nails" when checking</t>
   </si>
   <si>
@@ -765,6 +762,9 @@
   </si>
   <si>
     <t>not needed</t>
+  </si>
+  <si>
+    <t>NormalCount</t>
   </si>
 </sst>
 </file>
@@ -1283,7 +1283,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1311,7 +1311,7 @@
         <v>210</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G1" s="9"/>
     </row>
@@ -1415,7 +1415,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>211</v>
+        <v>240</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -1437,7 +1437,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>177</v>
@@ -1463,7 +1463,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -1632,191 +1632,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5B459A-3BB1-EB4C-924B-0D3FED2B4C76}">
-  <dimension ref="A1:D12"/>
-  <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>221</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="16" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="17" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
-      <c r="B4" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>210</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>239</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>224</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="D12" t="s">
-        <v>240</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44A7D45-3D37-034F-A1FB-B28B84ABA07F}">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="37.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>186</v>
-      </c>
-      <c r="B4" t="s">
-        <v>182</v>
-      </c>
-      <c r="C4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>183</v>
-      </c>
-      <c r="C6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16772568-7503-3B4E-B82C-A26E56E7827F}">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1852,7 +1673,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B3" s="5">
         <v>100</v>
@@ -1866,7 +1687,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B4" s="5">
         <v>50</v>
@@ -1883,7 +1704,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B5" s="2">
         <v>200</v>
@@ -1931,7 +1752,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B8" s="2">
         <v>0</v>
@@ -1940,29 +1761,29 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B10" s="2" t="b">
         <v>0</v>
@@ -1971,12 +1792,12 @@
         <v>208</v>
       </c>
       <c r="E10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B11" s="2" t="b">
         <v>1</v>
@@ -1985,10 +1806,10 @@
         <v>208</v>
       </c>
       <c r="D11" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E11" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -2048,12 +1869,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E766410-42AB-D842-913C-A2316B1EA100}">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2081,10 +1902,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2098,7 +1919,7 @@
         <v>171</v>
       </c>
       <c r="E3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2159,35 +1980,214 @@
         <v>200</v>
       </c>
       <c r="E8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B9" t="s">
         <v>210</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B10" t="s">
         <v>210</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D10" t="s">
-        <v>232</v>
+        <v>231</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5B459A-3BB1-EB4C-924B-0D3FED2B4C76}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="13"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="17" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="13"/>
+      <c r="B4" s="18" t="s">
+        <v>236</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
+      <c r="B5" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="12"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D12" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44A7D45-3D37-034F-A1FB-B28B84ABA07F}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C6" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -3009,6 +3009,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DA12DE6878FEE740AAE11B8EF5A3BEB8" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ccf3f071624932fa9b6b142dc8790e1c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bf33d030-a745-437b-8efe-493a0e84c7f1" xmlns:ns3="38766943-c6ee-43fb-a1f1-f050a673c741" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="46fa4806b78295368f283e4cef5efe23" ns2:_="" ns3:_="">
     <xsd:import namespace="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
@@ -3219,36 +3234,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030D8A7F-6A3B-4D41-86D3-C760184B49E7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A07F53CA-6B4E-4B2E-8600-AB0859BD2077}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
-    <ds:schemaRef ds:uri="38766943-c6ee-43fb-a1f1-f050a673c741"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3271,9 +3260,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A07F53CA-6B4E-4B2E-8600-AB0859BD2077}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{030D8A7F-6A3B-4D41-86D3-C760184B49E7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bf33d030-a745-437b-8efe-493a0e84c7f1"/>
+    <ds:schemaRef ds:uri="38766943-c6ee-43fb-a1f1-f050a673c741"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>